<commit_message>
identify transition bins and use ()
</commit_message>
<xml_diff>
--- a/FCOV_TEMPLATE.xlsx
+++ b/FCOV_TEMPLATE.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="79">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -254,6 +254,82 @@
   </si>
   <si>
     <t>none</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cp_rxpkt_len_trans</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MIN_MAX</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MAX_MIN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>64 =&gt; 1518</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1518 =&gt; 64</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cp_chipmode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MODE0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MODE1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2'b01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MODE2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2'b10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>illegal_bins</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MODE3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2'b11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>$</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -620,10 +696,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>
@@ -861,36 +937,67 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
       <c r="B17">
         <v>6</v>
       </c>
       <c r="C17" t="s">
+        <v>60</v>
+      </c>
+      <c r="D17" t="s">
+        <v>6</v>
+      </c>
+      <c r="G17" t="s">
+        <v>61</v>
+      </c>
+      <c r="H17" t="s">
+        <v>63</v>
+      </c>
+      <c r="I17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="G18" t="s">
+        <v>62</v>
+      </c>
+      <c r="H18" t="s">
+        <v>64</v>
+      </c>
+      <c r="I18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="B19">
+        <v>7</v>
+      </c>
+      <c r="C19" t="s">
         <v>36</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D19" t="s">
         <v>35</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F19" t="s">
         <v>43</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G19" t="s">
         <v>37</v>
       </c>
-      <c r="H17" t="s">
+      <c r="H19" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A19" t="s">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A21" t="s">
         <v>56</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C21" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A21" t="s">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A23" t="s">
         <v>54</v>
       </c>
     </row>
@@ -903,10 +1010,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>
@@ -917,7 +1024,7 @@
     <col min="4" max="4" width="54" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4.36328125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.90625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.36328125" customWidth="1"/>
     <col min="8" max="8" width="27.08984375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.54296875" customWidth="1"/>
     <col min="10" max="10" width="12.81640625" customWidth="1"/>
@@ -964,216 +1071,67 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>69</v>
       </c>
       <c r="G2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2">
-        <v>64</v>
+        <v>70</v>
+      </c>
+      <c r="H2" t="s">
+        <v>20</v>
       </c>
       <c r="I2" t="s">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="J2" t="s">
-        <v>46</v>
-      </c>
-      <c r="K2">
-        <v>1</v>
+        <v>65</v>
+      </c>
+      <c r="K2" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A3" s="2"/>
       <c r="G3" t="s">
-        <v>8</v>
+        <v>71</v>
       </c>
       <c r="H3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J3" t="s">
-        <v>47</v>
-      </c>
-      <c r="K3">
-        <v>10</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.4">
       <c r="G4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H4">
-        <v>1518</v>
+        <v>73</v>
+      </c>
+      <c r="H4" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="F5" t="s">
+        <v>75</v>
+      </c>
       <c r="G5" t="s">
-        <v>11</v>
+        <v>76</v>
       </c>
       <c r="H5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H6">
-        <v>6</v>
-      </c>
-      <c r="J6" t="s">
-        <v>48</v>
-      </c>
-      <c r="K6">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="G7" t="s">
-        <v>51</v>
-      </c>
-      <c r="H7" t="s">
-        <v>52</v>
-      </c>
-      <c r="J7" t="s">
-        <v>49</v>
-      </c>
-      <c r="K7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="B8">
-        <v>3</v>
-      </c>
-      <c r="C8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" t="s">
-        <v>18</v>
-      </c>
-      <c r="G8" t="s">
-        <v>19</v>
-      </c>
-      <c r="H8" t="s">
-        <v>20</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="G9" t="s">
-        <v>21</v>
-      </c>
-      <c r="H9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="G10" t="s">
-        <v>22</v>
-      </c>
-      <c r="H10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="G11" t="s">
-        <v>25</v>
-      </c>
-      <c r="H11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A12" t="s">
-        <v>57</v>
-      </c>
-      <c r="C12" t="s">
-        <v>58</v>
-      </c>
-      <c r="D12" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="B14">
-        <v>4</v>
-      </c>
-      <c r="C14" t="s">
-        <v>27</v>
-      </c>
-      <c r="D14" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="B15">
-        <v>5</v>
-      </c>
-      <c r="C15" t="s">
-        <v>29</v>
-      </c>
-      <c r="D15" t="s">
-        <v>30</v>
-      </c>
-      <c r="G15" t="s">
-        <v>31</v>
-      </c>
-      <c r="H15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="G16" t="s">
-        <v>32</v>
-      </c>
-      <c r="H16" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="B17">
-        <v>6</v>
-      </c>
-      <c r="C17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D17" t="s">
-        <v>35</v>
-      </c>
-      <c r="F17" t="s">
-        <v>43</v>
-      </c>
-      <c r="G17" t="s">
-        <v>37</v>
-      </c>
-      <c r="H17" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A19" t="s">
-        <v>56</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="A9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="C21" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A21" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A23" t="s">
         <v>54</v>
       </c>
     </row>

</xml_diff>